<commit_message>
[edit] Correo y reporte
Edicion del envio de correo y de la generacion del reporte de accesorios
</commit_message>
<xml_diff>
--- a/public/templateBajas.xlsx
+++ b/public/templateBajas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t># Activo</t>
   </si>
@@ -44,12 +44,15 @@
   <si>
     <t>Fecha de baja</t>
   </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -73,6 +76,12 @@
     <font>
       <b/>
       <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -217,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -232,13 +241,17 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
@@ -336,13 +349,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1876425</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
@@ -668,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,12 +693,12 @@
     <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" customWidth="1"/>
-    <col min="6" max="6" width="44.7109375" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
+    <col min="5" max="6" width="23.5703125" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -693,8 +706,9 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -702,8 +716,9 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -711,28 +726,30 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="1"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
       <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="1"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
       <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -740,8 +757,9 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -749,8 +767,9 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -758,8 +777,9 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -775,64 +795,75 @@
       <c r="E9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="3"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="9"/>
       <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="14"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="16"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
-    <mergeCell ref="C4:E5"/>
+    <mergeCell ref="D4:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>